<commit_message>
justdial stock result file updated
</commit_message>
<xml_diff>
--- a/LOT_MGMT/filtered_data.xlsx
+++ b/LOT_MGMT/filtered_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,12 +508,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23-05-2025</t>
+          <t>03-07-2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -528,18 +528,18 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="G2" t="n">
-        <v>80</v>
+        <v>927.5700000000001</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>10,000.47</t>
+          <t>46,378.28</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -549,27 +549,27 @@
         <v>3.6</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>46.45</v>
       </c>
       <c r="L2" t="n">
-        <v>1.51</v>
+        <v>0.05</v>
       </c>
       <c r="M2" t="n">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21-05-2025</t>
+          <t>02-07-2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -584,18 +584,18 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>750</v>
+        <v>50</v>
       </c>
       <c r="G3" t="n">
-        <v>79.54000000000001</v>
+        <v>917.5599999999999</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>59,651.73</t>
+          <t>45,877.92</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -605,27 +605,27 @@
         <v>3.6</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>45.8</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08</v>
+        <v>6.92</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15-05-2025</t>
+          <t>30-06-2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -640,18 +640,18 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>76.70999999999999</v>
+        <v>930.5599999999999</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>19,177.16</t>
+          <t>46,528.13</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -661,27 +661,27 @@
         <v>3.6</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>46.6</v>
       </c>
       <c r="L4" t="n">
-        <v>2.89</v>
+        <v>0.05</v>
       </c>
       <c r="M4" t="n">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15-05-2025</t>
+          <t>25-06-2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -700,44 +700,42 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>77.17</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>38,585.77</t>
-        </is>
+        <v>918.39</v>
+      </c>
+      <c r="H5" t="n">
+        <v>918.39</v>
       </c>
       <c r="I5" t="n">
-        <v>20</v>
+        <v>0.4</v>
       </c>
       <c r="J5" t="n">
-        <v>3.6</v>
+        <v>0.08</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>5.82</v>
+        <v>0.03</v>
       </c>
       <c r="M5" t="n">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12-05-2025</t>
+          <t>25-06-2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -756,44 +754,42 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>78.23</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>19,557.23</t>
-        </is>
+        <v>918.4400000000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>918.4400000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>20</v>
+        <v>0.4</v>
       </c>
       <c r="J6" t="n">
-        <v>3.6</v>
+        <v>0.08</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>2.95</v>
+        <v>0.03</v>
       </c>
       <c r="M6" t="n">
-        <v>351</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12-05-2025</t>
+          <t>25-06-2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -812,44 +808,44 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>500</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>79.19</v>
+        <v>918.38</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>39,595.97</t>
+          <t>1,836.75</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>0.8</v>
       </c>
       <c r="J7" t="n">
-        <v>3.6</v>
+        <v>0.14</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>5.97</v>
+        <v>0.06</v>
       </c>
       <c r="M7" t="n">
-        <v>351</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nip. India Gold</t>
+          <t>Just Dial</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>12-05-2025</t>
+          <t>25-06-2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -868,33 +864,2035 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="G8" t="n">
-        <v>78.72</v>
+        <v>918.38</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>9,840.43</t>
+          <t>10,102.22</t>
         </is>
       </c>
       <c r="I8" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="H9" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>918.34</v>
+      </c>
+      <c r="H10" t="n">
+        <v>918.34</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2,755.15</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="H12" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1,836.75</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2,755.15</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2,755.15</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>40</v>
+      </c>
+      <c r="G16" t="n">
+        <v>924.5700000000001</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>36,982.81</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>16</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K16" t="n">
+        <v>36.97</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2,755.15</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="H18" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="H20" t="n">
+        <v>918.39</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>12</v>
+      </c>
+      <c r="G21" t="n">
+        <v>918.4299999999999</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>11,021.19</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>40</v>
+      </c>
+      <c r="G22" t="n">
+        <v>913.15</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>36,525.83</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>20</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J22" t="n">
         <v>3.6</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="M8" t="n">
-        <v>351</v>
-      </c>
-      <c r="N8" t="n">
-        <v>125</v>
+      <c r="K22" t="n">
+        <v>9.24</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>918.38</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1,836.75</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="H24" t="n">
+        <v>918.4400000000001</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>10</v>
+      </c>
+      <c r="G25" t="n">
+        <v>925.26</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>9,252.62</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="K25" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>25-06-2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>60</v>
+      </c>
+      <c r="G26" t="n">
+        <v>933.65</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>56,018.89</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>20</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K26" t="n">
+        <v>55.46</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16-06-2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>10</v>
+      </c>
+      <c r="G27" t="n">
+        <v>873.4</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>8,733.97</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>20</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K27" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>16-06-2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>10</v>
+      </c>
+      <c r="G28" t="n">
+        <v>883.4</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>8,833.98</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>20</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K28" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13-06-2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>20</v>
+      </c>
+      <c r="G29" t="n">
+        <v>892.24</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>17,844.72</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>20</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K29" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>50</v>
+      </c>
+      <c r="G30" t="n">
+        <v>912.55</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>45,627.62</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>20</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K30" t="n">
+        <v>45.55</v>
+      </c>
+      <c r="L30" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>11-06-2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>44</v>
+      </c>
+      <c r="G31" t="n">
+        <v>921.5599999999999</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>40,548.77</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="J31" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="K31" t="n">
+        <v>40.48</v>
+      </c>
+      <c r="L31" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11-06-2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>6</v>
+      </c>
+      <c r="G32" t="n">
+        <v>921.5599999999999</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>5,529.38</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="K32" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>09-06-2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>10</v>
+      </c>
+      <c r="G33" t="n">
+        <v>910</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>9,100.04</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K33" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>09-06-2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>90</v>
+      </c>
+      <c r="G34" t="n">
+        <v>909.3200000000001</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>81,838.80</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>18</v>
+      </c>
+      <c r="J34" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="K34" t="n">
+        <v>81.98999999999999</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>09-06-2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>10</v>
+      </c>
+      <c r="G35" t="n">
+        <v>918.42</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>9,184.19</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>20</v>
+      </c>
+      <c r="J35" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>06-06-2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>28</v>
+      </c>
+      <c r="G36" t="n">
+        <v>908.59</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>25,440.46</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K36" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>06-06-2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>72</v>
+      </c>
+      <c r="G37" t="n">
+        <v>908.59</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>65,418.36</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="K37" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>06-06-2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" t="n">
+        <v>900.39</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>7,203.16</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>06-06-2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>55</v>
+      </c>
+      <c r="G39" t="n">
+        <v>907.91</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>49,935.03</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="K39" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>06-06-2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>92</v>
+      </c>
+      <c r="G40" t="n">
+        <v>900.4</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>82,836.40</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>05-06-2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>50</v>
+      </c>
+      <c r="G41" t="n">
+        <v>900.59</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>45,029.67</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>20</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K41" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>04-06-2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>27</v>
+      </c>
+      <c r="G42" t="n">
+        <v>889.52</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>24,017.17</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="K42" t="n">
+        <v>23.98</v>
+      </c>
+      <c r="L42" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>04-06-2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>8</v>
+      </c>
+      <c r="G43" t="n">
+        <v>889.53</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>7,116.21</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="K43" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Just Dial</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>04-06-2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>15</v>
+      </c>
+      <c r="G44" t="n">
+        <v>889.53</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>13,342.89</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>6</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="K44" t="n">
+        <v>13.32</v>
+      </c>
+      <c r="L44" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VBL LOT PROFILING IS DONE
</commit_message>
<xml_diff>
--- a/LOT_MGMT/filtered_data.xlsx
+++ b/LOT_MGMT/filtered_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,12 +508,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>02-07-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -528,33 +528,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1,279.07</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>25,581.30</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H2" t="n">
+        <v>467.63</v>
       </c>
       <c r="I2" t="n">
-        <v>20</v>
+        <v>0.33</v>
       </c>
       <c r="J2" t="n">
-        <v>3.6</v>
+        <v>0.06</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -566,12 +562,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>02-07-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -590,29 +586,25 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1,278.45</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>25,569.08</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H3" t="n">
+        <v>467.63</v>
       </c>
       <c r="I3" t="n">
-        <v>20</v>
+        <v>0.33</v>
       </c>
       <c r="J3" t="n">
-        <v>3.6</v>
+        <v>0.06</v>
       </c>
       <c r="K3" t="n">
-        <v>6.39</v>
+        <v>0.47</v>
       </c>
       <c r="L3" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -624,12 +616,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>01-07-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -644,50 +636,48 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1,281.40</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="G4" t="n">
+        <v>467.62</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>11,532.57</t>
+          <t>7,481.94</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>5.33</v>
       </c>
       <c r="J4" t="n">
-        <v>1.62</v>
+        <v>0.96</v>
       </c>
       <c r="K4" t="n">
-        <v>11.51</v>
+        <v>7.5</v>
       </c>
       <c r="L4" t="n">
-        <v>1.74</v>
+        <v>0.01</v>
       </c>
       <c r="M4" t="n">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01-07-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -702,50 +692,46 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>11</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1,281.40</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>14,095.37</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H5" t="n">
+        <v>467.63</v>
       </c>
       <c r="I5" t="n">
-        <v>11</v>
+        <v>0.33</v>
       </c>
       <c r="J5" t="n">
-        <v>1.98</v>
+        <v>0.06</v>
       </c>
       <c r="K5" t="n">
-        <v>14.07</v>
+        <v>0.47</v>
       </c>
       <c r="L5" t="n">
-        <v>2.12</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>20-06-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -764,26 +750,24 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1,198.58</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>467.62</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1,198.58</t>
+          <t>2,338.10</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>1.67</v>
       </c>
       <c r="J6" t="n">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="K6" t="n">
-        <v>1.2</v>
+        <v>2.34</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -798,12 +782,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20-06-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -822,29 +806,27 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>19</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1,198.58</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>467.62</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>22,772.94</t>
+          <t>1,402.87</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>3.42</v>
+        <v>0.18</v>
       </c>
       <c r="K7" t="n">
-        <v>22.82</v>
+        <v>1.41</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -856,12 +838,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18-06-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -876,50 +858,48 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1,187.53</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="G8" t="n">
+        <v>467.62</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5,937.63</t>
+          <t>6,546.69</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>20</v>
+        <v>4.67</v>
       </c>
       <c r="J8" t="n">
-        <v>3.6</v>
+        <v>0.84</v>
       </c>
       <c r="K8" t="n">
-        <v>5.91</v>
+        <v>6.56</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9</v>
+        <v>0.01</v>
       </c>
       <c r="M8" t="n">
-        <v>349</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Max Healthcare</t>
+          <t>Varun Beverages</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>09-06-2025</t>
+          <t>15-07-2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -938,34 +918,2374 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1,181.41</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>11,814.13</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H9" t="n">
+        <v>467.63</v>
       </c>
       <c r="I9" t="n">
-        <v>20</v>
+        <v>0.33</v>
       </c>
       <c r="J9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>15-07-2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>16</v>
+      </c>
+      <c r="G10" t="n">
+        <v>467.62</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>7,481.94</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="K10" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>15-07-2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H11" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>15-07-2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="H12" t="n">
+        <v>467.63</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19-06-2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" t="n">
+        <v>453.32</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>13,599.68</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" t="n">
         <v>3.6</v>
       </c>
-      <c r="K9" t="n">
-        <v>11.85</v>
-      </c>
-      <c r="L9" t="n">
+      <c r="K13" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="M13" t="n">
+        <v>337</v>
+      </c>
+      <c r="N13" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16-06-2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>30</v>
+      </c>
+      <c r="G14" t="n">
+        <v>463.33</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>13,900.04</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>20</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K14" t="n">
+        <v>13.86</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="M14" t="n">
+        <v>334</v>
+      </c>
+      <c r="N14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>13-06-2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" t="n">
+        <v>468.88</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2,813.27</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M15" t="n">
+        <v>331</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>13-06-2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>44</v>
+      </c>
+      <c r="G16" t="n">
+        <v>468.88</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>20,630.57</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="K16" t="n">
+        <v>20.59</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="M16" t="n">
+        <v>331</v>
+      </c>
+      <c r="N16" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" t="n">
+        <v>482.65</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>9,652.93</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.01</v>
       </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>20</v>
+      </c>
+      <c r="G18" t="n">
+        <v>479.21</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>9,584.24</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>20</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>83</v>
+      </c>
+      <c r="G19" t="n">
+        <v>482.29</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>40,029.75</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="K19" t="n">
+        <v>39.99</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G20" t="n">
+        <v>477.42</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>9,548.41</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>20</v>
+      </c>
+      <c r="J20" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K20" t="n">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" t="n">
+        <v>482.29</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>3,376.02</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11-06-2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>50</v>
+      </c>
+      <c r="G22" t="n">
+        <v>471.03</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>23,551.50</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>20</v>
+      </c>
+      <c r="J22" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K22" t="n">
+        <v>23.53</v>
+      </c>
+      <c r="L22" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="M22" t="n">
+        <v>329</v>
+      </c>
+      <c r="N22" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11-06-2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>20</v>
+      </c>
+      <c r="G23" t="n">
+        <v>473.74</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>9,474.78</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>20</v>
+      </c>
+      <c r="J23" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K23" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="M23" t="n">
+        <v>329</v>
+      </c>
+      <c r="N23" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10-06-2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>30</v>
+      </c>
+      <c r="G24" t="n">
+        <v>482.03</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>14,460.88</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>12</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="K24" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10-06-2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>20</v>
+      </c>
+      <c r="G25" t="n">
+        <v>482.39</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>9,647.79</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>8</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="K25" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10-06-2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>20</v>
+      </c>
+      <c r="G26" t="n">
+        <v>478.21</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>9,564.24</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>20</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>04-06-2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>50</v>
+      </c>
+      <c r="G27" t="n">
+        <v>469.03</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>23,451.34</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>20</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K27" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="L27" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="M27" t="n">
+        <v>322</v>
+      </c>
+      <c r="N27" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>22-05-2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>20</v>
+      </c>
+      <c r="G28" t="n">
+        <v>474.64</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>9,492.83</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>20</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K28" t="n">
+        <v>9.460000000000001</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="M28" t="n">
+        <v>309</v>
+      </c>
+      <c r="N28" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>20-05-2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>30</v>
+      </c>
+      <c r="G29" t="n">
+        <v>493.36</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>14,800.92</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>20</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K29" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="M29" t="n">
+        <v>307</v>
+      </c>
+      <c r="N29" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>20-05-2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>30</v>
+      </c>
+      <c r="G30" t="n">
+        <v>488.36</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>14,650.89</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>20</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K30" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M30" t="n">
+        <v>307</v>
+      </c>
+      <c r="N30" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>20-05-2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>50</v>
+      </c>
+      <c r="G31" t="n">
+        <v>483.05</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>24,152.38</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>20</v>
+      </c>
+      <c r="J31" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K31" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="L31" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="M31" t="n">
+        <v>307</v>
+      </c>
+      <c r="N31" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>16-05-2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>50</v>
+      </c>
+      <c r="G32" t="n">
+        <v>499.07</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>24,953.29</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>20</v>
+      </c>
+      <c r="J32" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K32" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="L32" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="M32" t="n">
+        <v>303</v>
+      </c>
+      <c r="N32" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>16-05-2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>50</v>
+      </c>
+      <c r="G33" t="n">
+        <v>504.97</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>25,248.35</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>20</v>
+      </c>
+      <c r="J33" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K33" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="L33" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>12-05-2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>200</v>
+      </c>
+      <c r="G34" t="n">
+        <v>510.35</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>1,02,070.50</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>20</v>
+      </c>
+      <c r="J34" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K34" t="n">
+        <v>102.2</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>09-05-2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>35</v>
+      </c>
+      <c r="G35" t="n">
+        <v>479.5</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>16,782.64</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>14</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>09-05-2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>50</v>
+      </c>
+      <c r="G36" t="n">
+        <v>495.39</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>24,769.41</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>20</v>
+      </c>
+      <c r="J36" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K36" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>09-05-2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>15</v>
+      </c>
+      <c r="G37" t="n">
+        <v>479.5</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>7,192.56</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>6</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08-05-2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>50</v>
+      </c>
+      <c r="G38" t="n">
+        <v>493.06</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>24,653.03</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>20</v>
+      </c>
+      <c r="J38" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K38" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="L38" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08-05-2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>50</v>
+      </c>
+      <c r="G39" t="n">
+        <v>503.06</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>25,153.14</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>20</v>
+      </c>
+      <c r="J39" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K39" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="L39" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08-05-2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>50</v>
+      </c>
+      <c r="G40" t="n">
+        <v>498.06</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>24,903.08</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>20</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K40" t="n">
+        <v>24.85</v>
+      </c>
+      <c r="L40" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>07-05-2025</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>50</v>
+      </c>
+      <c r="G41" t="n">
+        <v>507.07</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>25,353.71</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>20</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K41" t="n">
+        <v>25.39</v>
+      </c>
+      <c r="L41" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>07-05-2025</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>30</v>
+      </c>
+      <c r="G42" t="n">
+        <v>512.39</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>15,371.70</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>20</v>
+      </c>
+      <c r="J42" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K42" t="n">
+        <v>15.24</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>07-05-2025</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>INTERIM DIVIDEND</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>105</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H43" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>06-05-2025</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>30</v>
+      </c>
+      <c r="G44" t="n">
+        <v>517.4</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>15,521.96</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>20</v>
+      </c>
+      <c r="J44" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K44" t="n">
+        <v>15.48</v>
+      </c>
+      <c r="L44" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>02-05-2025</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>40</v>
+      </c>
+      <c r="G45" t="n">
+        <v>522.86</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>20,914.36</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>20</v>
+      </c>
+      <c r="J45" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K45" t="n">
+        <v>20.87</v>
+      </c>
+      <c r="L45" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>25-04-2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>30</v>
+      </c>
+      <c r="G46" t="n">
+        <v>526.71</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>15,801.29</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>20</v>
+      </c>
+      <c r="J46" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K46" t="n">
+        <v>15.76</v>
+      </c>
+      <c r="L46" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>17-04-2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>50</v>
+      </c>
+      <c r="G47" t="n">
+        <v>562.34</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>28,117.20</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>20</v>
+      </c>
+      <c r="J47" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K47" t="n">
+        <v>28.17</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>08-04-2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>20</v>
+      </c>
+      <c r="G48" t="n">
+        <v>538.26</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>10,765.21</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>20</v>
+      </c>
+      <c r="J48" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K48" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07-04-2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>20</v>
+      </c>
+      <c r="G49" t="n">
+        <v>509.58</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>10,191.65</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>20</v>
+      </c>
+      <c r="J49" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K49" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="L49" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>04-04-2025</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>FINAL DIVIDEND</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>25</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H50" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Varun Beverages</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>04-04-2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Axisdirect</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>30</v>
+      </c>
+      <c r="G51" t="n">
+        <v>537.47</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>16,124.17</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>20</v>
+      </c>
+      <c r="J51" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K51" t="n">
+        <v>16.08</v>
+      </c>
+      <c r="L51" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>